<commit_message>
Updated graphs and correlations
</commit_message>
<xml_diff>
--- a/datasets/meat.xlsx
+++ b/datasets/meat.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\covid-19-india\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\covid-19-prediction\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336316BD-B8AA-4C8C-BC03-09E15B6E628A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28155245-97D6-47AE-99DE-76D892FBA2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6410" yWindow="5520" windowWidth="22050" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12370" yWindow="5180" windowWidth="22050" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>[11]</t>
   </si>
@@ -387,9 +393,6 @@
     <t>Namibia</t>
   </si>
   <si>
-    <t xml:space="preserve">  Nepal</t>
-  </si>
-  <si>
     <t>Netherlands</t>
   </si>
   <si>
@@ -528,9 +531,6 @@
     <t>Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve"> Switzerland</t>
-  </si>
-  <si>
     <t>Syria</t>
   </si>
   <si>
@@ -570,9 +570,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>United States of America</t>
-  </si>
-  <si>
     <t>United States Virgin Islands</t>
   </si>
   <si>
@@ -598,6 +595,18 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -915,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2202,7 +2211,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="B119">
         <v>10</v>
@@ -2213,7 +2222,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B120">
         <v>89.3</v>
@@ -2224,7 +2233,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B121">
         <v>73.3</v>
@@ -2235,7 +2244,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B122">
         <v>76.599999999999994</v>
@@ -2246,7 +2255,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>142.1</v>
@@ -2257,7 +2266,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B124">
         <v>14.9</v>
@@ -2268,7 +2277,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B125">
         <v>11.2</v>
@@ -2279,7 +2288,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B126">
         <v>8.6</v>
@@ -2290,7 +2299,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B127">
         <v>61.7</v>
@@ -2301,7 +2310,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B128">
         <v>10.8</v>
@@ -2312,7 +2321,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B129">
         <v>49.8</v>
@@ -2320,7 +2329,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B130">
         <v>12.3</v>
@@ -2331,7 +2340,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131">
         <v>54.5</v>
@@ -2342,7 +2351,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132">
         <v>73</v>
@@ -2350,7 +2359,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133">
         <v>70.3</v>
@@ -2361,7 +2370,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B134">
         <v>34.5</v>
@@ -2372,7 +2381,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B135">
         <v>31.1</v>
@@ -2383,7 +2392,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B136">
         <v>78.099999999999994</v>
@@ -2394,7 +2403,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137">
         <v>91.1</v>
@@ -2405,7 +2414,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138">
         <v>90.5</v>
@@ -2413,7 +2422,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139">
         <v>46.8</v>
@@ -2421,7 +2430,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140">
         <v>54.5</v>
@@ -2432,7 +2441,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141">
         <v>51</v>
@@ -2443,7 +2452,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142">
         <v>4.4000000000000004</v>
@@ -2454,7 +2463,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143">
         <v>99.3</v>
@@ -2465,7 +2474,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144">
         <v>124.1</v>
@@ -2476,7 +2485,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B145">
         <v>79.099999999999994</v>
@@ -2487,7 +2496,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146">
         <v>82.6</v>
@@ -2498,7 +2507,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B147">
         <v>9.6</v>
@@ -2509,7 +2518,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B148">
         <v>44.6</v>
@@ -2520,7 +2529,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B149">
         <v>17.7</v>
@@ -2531,7 +2540,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C150">
         <v>45.2</v>
@@ -2539,7 +2548,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B151">
         <v>77.599999999999994</v>
@@ -2550,7 +2559,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B152">
         <v>51.1</v>
@@ -2561,7 +2570,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B153">
         <v>6.1</v>
@@ -2572,7 +2581,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B154">
         <v>71.099999999999994</v>
@@ -2580,7 +2589,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B155">
         <v>67.400000000000006</v>
@@ -2591,7 +2600,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B156">
         <v>88</v>
@@ -2602,7 +2611,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B157">
         <v>9.6999999999999993</v>
@@ -2613,7 +2622,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B158">
         <v>39</v>
@@ -2624,7 +2633,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B159">
         <v>48</v>
@@ -2635,7 +2644,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B160">
         <v>118.6</v>
@@ -2646,7 +2655,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B161">
         <v>6.6</v>
@@ -2657,7 +2666,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B162">
         <v>21</v>
@@ -2668,7 +2677,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B163">
         <v>40.299999999999997</v>
@@ -2679,7 +2688,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B164">
         <v>34.200000000000003</v>
@@ -2690,7 +2699,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B165">
         <v>76.099999999999994</v>
@@ -2701,7 +2710,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="B166">
         <v>72.900000000000006</v>
@@ -2712,7 +2721,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B167">
         <v>21.2</v>
@@ -2723,7 +2732,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B168">
         <v>8.6999999999999993</v>
@@ -2734,7 +2743,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B169">
         <v>27.9</v>
@@ -2745,7 +2754,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B170">
         <v>41.3</v>
@@ -2756,7 +2765,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B171">
         <v>10</v>
@@ -2778,7 +2787,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>57.8</v>
@@ -2789,7 +2798,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>25.5</v>
@@ -2800,7 +2809,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>19.3</v>
@@ -2811,7 +2820,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>41.7</v>
@@ -2822,7 +2831,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>11.7</v>
@@ -2833,7 +2842,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B178">
         <v>32.299999999999997</v>
@@ -2844,7 +2853,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B179">
         <v>74.400000000000006</v>
@@ -2855,7 +2864,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>79.599999999999994</v>
@@ -2866,7 +2875,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B181">
         <v>124.8</v>
@@ -2877,7 +2886,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B182">
         <v>6.6</v>
@@ -2885,7 +2894,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B183">
         <v>98.6</v>
@@ -2896,7 +2905,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B184">
         <v>20.7</v>
@@ -2907,7 +2916,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B185">
         <v>32.6</v>
@@ -2918,7 +2927,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B186">
         <v>56.6</v>
@@ -2929,7 +2938,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B187">
         <v>28.6</v>
@@ -2940,7 +2949,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B188">
         <v>14.7</v>
@@ -2951,7 +2960,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B189">
         <v>11.9</v>
@@ -2962,13 +2971,24 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B190">
         <v>15.2</v>
       </c>
       <c r="C190">
         <v>21.3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191">
+        <v>41.3</v>
+      </c>
+      <c r="C191">
+        <v>41.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>